<commit_message>
fix: convert float64 column to object to prevent assignment crash
</commit_message>
<xml_diff>
--- a/ActiveRoaster.xlsx
+++ b/ActiveRoaster.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="SS 1Q" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -436,4 +437,1157 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D70"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>1st CA</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total Score</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Abdul Azeez Haliyah</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Abdul Hammed Qowiyat</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Abdul Kareem Zainab</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Abdul Quadri Faridah</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Abdulmumin Soburat</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Adeaga Mercy</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Adebayo Faouziyah</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Adekola Ayomide</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Adekunle Favour</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Adesina Adeola</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Ajao Lois</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Ajayi Elizabeth</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ajayi Temilade</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Ajetunmobi Hepzibah</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Akindele Faith</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Akinlekan Faith</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Akinlolu Oluwademilade</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Akpan Priscilla</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Alade Pelumi</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>8</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Alaka Courage</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Alli Oluwadarasimi</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Asalu Rukayat</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Asiwaju Alimat</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Atolagbe Deborah</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Bamgbose Faridah</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Bamigbola Fiyinfoluwa</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Bashiru Aishat</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Bello Azeezat</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Benjamin Victoria</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Daniel Oluwadarasimi</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Durodola Naimot</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Edegbai Joy</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Fafowora Mofeyisara</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Fayemi Sunmisola</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Hammed Uruwat</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Hamzat Darasimi</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Ibrahim Yussiroh</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Ilori Julianah</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Jimoh Davida</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Jose Olayinka</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Joshua Tamilore</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>9</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Kazeem Alimot</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Kolawole Pemisire</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Lawal Aramide</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Lukman Ayomikun</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Morakinyo Eniola</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Moshood Zainab</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Nurudeen Moridyyah</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Obasuyi Peculiar</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Odesola Suudat</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Okanlawon Esther</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Okeowo Sofiat</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Oladimeji Adijat</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Oladokun Haliyah</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Olaniyi Latifat</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Olanrewaju  Aishat</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Olateju Iyanuoluwa</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Olatunde Abigeal</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Olayanju Oluwasikemi</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Olayiwola Fathia</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Oluokun Favor</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Oluwagbenga Deborah</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Oluwasola Oluwaseyifunmi</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Oluwatoyin Jewel</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Oluyemi Oluwadarasimi</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Oriade Bolade</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Salami Oluwatobi</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Unorbueze Victoria</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Uzogbo Chioma</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Pre-upgrade snapshot: current working state before 3D UI/UX premium upgrade
</commit_message>
<xml_diff>
--- a/ActiveRoaster.xlsx
+++ b/ActiveRoaster.xlsx
@@ -7,8 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="General" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="SS 1Q" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="1A" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Class1A" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SS 1Q - Uncategorized" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SS 2A" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="SS1Q" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Test Class" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,9 +432,18 @@
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Class</t>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Student A</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Student B</t>
         </is>
       </c>
     </row>
@@ -445,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,65 +472,137 @@
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>1st CA</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Total Score</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Position</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Abdul Azeez Haliyah</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3rd</t>
+          <t>Student A</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Abdul Hammed Qowiyat</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>3rd</t>
+          <t>Student B</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>1st CA</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Total Score</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Adekunle Favour</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SS 1Q</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Akindele Faith Oluwalonimi</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SS 1Q</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1st</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Abdul Kareem Zainab</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="inlineStr">
+          <t>Bamigbola Fiyinfoluwa</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SS 1Q</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -526,30 +611,48 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Abdul Quadri Faridah</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>3rd</t>
+          <t>Benjamin Victoria</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SS 1Q</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>9th</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Abdulmumin Soburat</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="inlineStr">
+          <t>Fayemi Sunmisola</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SS 1Q</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -558,14 +661,23 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Adeaga Mercy</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="inlineStr">
+          <t>Joshua = Tamilore</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SS 1Q</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>7</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -574,30 +686,48 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Adebayo Faouziyah</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>3rd</t>
+          <t>Moshood Zainab</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SS 1Q</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>8th</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Adekola Ayomide</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="inlineStr">
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SS 1Q</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -606,32 +736,214 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Adekunle Favour</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="n">
+          <t>Oladokun Haliyale Adunni</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SS 1Q</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>0</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>3rd</t>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>10th</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Unorbueze Victoria</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SS 1Q</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>7</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mary</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Peter</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Student A</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Student B</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Student C</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A70"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Abdul Azeez Haliyah</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Abdul Hammed Qowiyat</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Abdul Kareem Zainab</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Abdul Quadri Faridah</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Abdulmumin Soburat</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Adeaga Mercy</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Adebayo Faouziyah</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Adekola Ayomide</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Adekunle Favour</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>Adesina Adeola</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>3rd</t>
         </is>
       </c>
     </row>
@@ -641,15 +953,6 @@
           <t>Ajao Lois</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -657,15 +960,6 @@
           <t>Ajayi Elizabeth</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -673,15 +967,6 @@
           <t>Ajayi Temilade</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -689,15 +974,6 @@
           <t>Ajetunmobi Hepzibah</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -705,15 +981,6 @@
           <t>Akindele Faith</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -721,15 +988,6 @@
           <t>Akinlekan Faith</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -737,15 +995,6 @@
           <t>Akinlolu Oluwademilade</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -753,15 +1002,6 @@
           <t>Akpan Priscilla</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -769,19 +1009,6 @@
           <t>Alade Pelumi</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>8</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -789,15 +1016,6 @@
           <t>Alaka Courage</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -805,15 +1023,6 @@
           <t>Alli Oluwadarasimi</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -821,15 +1030,6 @@
           <t>Asalu Rukayat</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -837,15 +1037,6 @@
           <t>Asiwaju Alimat</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -853,15 +1044,6 @@
           <t>Atolagbe Deborah</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -869,15 +1051,6 @@
           <t>Bamgbose Faridah</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -885,15 +1058,6 @@
           <t>Bamigbola Fiyinfoluwa</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -901,15 +1065,6 @@
           <t>Bashiru Aishat</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -917,15 +1072,6 @@
           <t>Bello Azeezat</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -933,15 +1079,6 @@
           <t>Benjamin Victoria</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -949,15 +1086,6 @@
           <t>Daniel Oluwadarasimi</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -965,15 +1093,6 @@
           <t>Durodola Naimot</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr"/>
-      <c r="C32" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -981,15 +1100,6 @@
           <t>Edegbai Joy</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr"/>
-      <c r="C33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -997,15 +1107,6 @@
           <t>Fafowora Mofeyisara</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1013,15 +1114,6 @@
           <t>Fayemi Sunmisola</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr"/>
-      <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1029,15 +1121,6 @@
           <t>Hammed Uruwat</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr"/>
-      <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1045,15 +1128,6 @@
           <t>Hamzat Darasimi</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr"/>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1061,15 +1135,6 @@
           <t>Ibrahim Yussiroh</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1077,15 +1142,6 @@
           <t>Ilori Julianah</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr"/>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1093,15 +1149,6 @@
           <t>Jimoh Davida</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr"/>
-      <c r="C40" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1109,15 +1156,6 @@
           <t>Jose Olayinka</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr"/>
-      <c r="C41" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1125,19 +1163,6 @@
           <t>Joshua Tamilore</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>9</v>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1145,15 +1170,6 @@
           <t>Kazeem Alimot</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr"/>
-      <c r="C43" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1161,15 +1177,6 @@
           <t>Kolawole Pemisire</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1177,15 +1184,6 @@
           <t>Lawal Aramide</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1193,15 +1191,6 @@
           <t>Lukman Ayomikun</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1209,15 +1198,6 @@
           <t>Morakinyo Eniola</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1225,15 +1205,6 @@
           <t>Moshood Zainab</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="n">
-        <v>0</v>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1241,15 +1212,6 @@
           <t>Nurudeen Moridyyah</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1257,15 +1219,6 @@
           <t>Obasuyi Peculiar</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr"/>
-      <c r="C50" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1273,15 +1226,6 @@
           <t>Odesola Suudat</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1289,15 +1233,6 @@
           <t>Okanlawon Esther</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1305,15 +1240,6 @@
           <t>Okeowo Sofiat</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr"/>
-      <c r="C53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1321,15 +1247,6 @@
           <t>Oladimeji Adijat</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr"/>
-      <c r="C54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1337,15 +1254,6 @@
           <t>Oladokun Haliyah</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1353,15 +1261,6 @@
           <t>Olaniyi Latifat</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1369,15 +1268,6 @@
           <t>Olanrewaju  Aishat</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1385,15 +1275,6 @@
           <t>Olateju Iyanuoluwa</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr"/>
-      <c r="C58" t="n">
-        <v>0</v>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1401,15 +1282,6 @@
           <t>Olatunde Abigeal</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="n">
-        <v>0</v>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1417,15 +1289,6 @@
           <t>Olayanju Oluwasikemi</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr"/>
-      <c r="C60" t="n">
-        <v>0</v>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1433,15 +1296,6 @@
           <t>Olayiwola Fathia</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1449,15 +1303,6 @@
           <t>Oluokun Favor</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr"/>
-      <c r="C62" t="n">
-        <v>0</v>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1465,15 +1310,6 @@
           <t>Oluwagbenga Deborah</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr"/>
-      <c r="C63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1481,15 +1317,6 @@
           <t>Oluwasola Oluwaseyifunmi</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="n">
-        <v>0</v>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1497,15 +1324,6 @@
           <t>Oluwatoyin Jewel</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="n">
-        <v>0</v>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1513,15 +1331,6 @@
           <t>Oluyemi Oluwadarasimi</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr"/>
-      <c r="C66" t="n">
-        <v>0</v>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1529,15 +1338,6 @@
           <t>Oriade Bolade</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr"/>
-      <c r="C67" t="n">
-        <v>0</v>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1545,15 +1345,6 @@
           <t>Salami Oluwatobi</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr"/>
-      <c r="C68" t="n">
-        <v>0</v>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1561,15 +1352,6 @@
           <t>Unorbueze Victoria</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr"/>
-      <c r="C69" t="n">
-        <v>0</v>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1577,13 +1359,58 @@
           <t>Uzogbo Chioma</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr"/>
-      <c r="C70" t="n">
-        <v>0</v>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>3rd</t>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Student A</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Student B</t>
         </is>
       </c>
     </row>

</xml_diff>